<commit_message>
ajout d'une colonne Ville
</commit_message>
<xml_diff>
--- a/data_aeroports.xlsx
+++ b/data_aeroports.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\utilisateur\Documents\Certif_Agile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3C0598D-216F-4AFD-9F3C-980168D2B80F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7EB5EEC-E0CC-4079-8BD5-3FF9BBF90A09}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{9B548A2A-51E3-42C3-BC03-87406874C064}"/>
   </bookViews>
@@ -25,11 +25,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t>Lyon Bron</t>
   </si>
   <si>
+    <t>Longvic</t>
+  </si>
+  <si>
+    <t>Valence</t>
+  </si>
+  <si>
     <t>La Rochelle</t>
   </si>
   <si>
@@ -118,6 +124,15 @@
   </si>
   <si>
     <t>1783*30</t>
+  </si>
+  <si>
+    <t>Ville</t>
+  </si>
+  <si>
+    <t>Lyon</t>
+  </si>
+  <si>
+    <t>Nancy</t>
   </si>
 </sst>
 </file>
@@ -174,15 +189,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BBB72A9C-0236-484C-84CD-CB4551274917}" name="Tableau1" displayName="Tableau1" ref="A1:F7" totalsRowShown="0">
-  <autoFilter ref="A1:F7" xr:uid="{5811B69B-6B9E-4D8A-BC1A-A6FF3B5B5FF7}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BBB72A9C-0236-484C-84CD-CB4551274917}" name="Tableau1" displayName="Tableau1" ref="A1:G7" totalsRowShown="0">
+  <autoFilter ref="A1:G7" xr:uid="{5811B69B-6B9E-4D8A-BC1A-A6FF3B5B5FF7}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{6A1CE787-F341-4C28-8F71-904D5E9FBF62}" name="Aéroport"/>
     <tableColumn id="2" xr3:uid="{675554F2-0496-44E4-8CEE-6BCE23A2EB93}" name="Altitude (pieds)"/>
     <tableColumn id="3" xr3:uid="{B614B8FF-6CCF-431C-A2E8-F13A57F82FB0}" name="Lat"/>
     <tableColumn id="4" xr3:uid="{5DDF6992-8E94-4B35-B5A2-F2D8941F67A8}" name="Lon"/>
     <tableColumn id="5" xr3:uid="{1BE3B49A-5F0B-45F2-AAFE-26DDB538E72D}" name="Dimensions Piste (mètres)"/>
     <tableColumn id="6" xr3:uid="{D67F0717-246B-4F6A-AF16-FFFD2C2184A2}" name="Nature piste"/>
+    <tableColumn id="7" xr3:uid="{902F46C8-EC84-4B07-8680-C5D2702F6169}" name="Ville"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -485,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{530278A2-638F-4A7F-B042-D2246EF587A4}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -498,27 +514,30 @@
     <col min="6" max="6" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -526,122 +545,141 @@
         <v>659</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <v>728</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
+      <c r="G3" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B4">
         <v>757</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>525</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B6">
         <v>74</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
         <v>27</v>
       </c>
-      <c r="E6" t="s">
-        <v>25</v>
-      </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>201</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="G7" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>